<commit_message>
Updated page classes and test class
</commit_message>
<xml_diff>
--- a/src/test/resources/ISP_DatabaseTestData.xlsx
+++ b/src/test/resources/ISP_DatabaseTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nishant\IdeaProjects\wd3seleniumcoopframework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCBD2BF-6A2D-4D31-85C1-B1474D3A4AE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CF77EFD-217C-47C2-8CBB-A4ED1763C14E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="GeneralInfo" sheetId="2" r:id="rId2"/>
-    <sheet name="AIEducationGoals" sheetId="3" r:id="rId3"/>
+    <sheet name="AdditionalInfo" sheetId="3" r:id="rId3"/>
+    <sheet name="SearchStudent" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="143">
   <si>
     <t>training@pragra.co</t>
   </si>
@@ -276,6 +277,191 @@
   </si>
   <si>
     <t>28-June-2014</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Shiva</t>
+  </si>
+  <si>
+    <t>Parent/Agent Email</t>
+  </si>
+  <si>
+    <t>Who should the school Invoice?</t>
+  </si>
+  <si>
+    <t>What email address should the Invoice be sent to?</t>
+  </si>
+  <si>
+    <t>Method of interview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I.D. </t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>I.D of Social Media</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>Fee Invoice</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Animals</t>
+  </si>
+  <si>
+    <t>Medications</t>
+  </si>
+  <si>
+    <t>Insects</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>HealthConcernExp  If yes, please explain:</t>
+  </si>
+  <si>
+    <t>MentalExp  If yes, please explain:</t>
+  </si>
+  <si>
+    <t>ConcernLifeExpl If yes, please explain:</t>
+  </si>
+  <si>
+    <t>medication regularly If yes, please describe:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of last Tetanus shot:_x000D_
+</t>
+  </si>
+  <si>
+    <t>If any of the above applies, please provide dates of illness:</t>
+  </si>
+  <si>
+    <t>If any of the above applies, please provide more information:</t>
+  </si>
+  <si>
+    <t>other medical conditions we should be aware of</t>
+  </si>
+  <si>
+    <t>If yes, please describe:</t>
+  </si>
+  <si>
+    <t>Please list any other health issues:</t>
+  </si>
+  <si>
+    <t>Family Doctor Name</t>
+  </si>
+  <si>
+    <t>Family Doctor Phone Number</t>
+  </si>
+  <si>
+    <t>Family Dentist Name</t>
+  </si>
+  <si>
+    <t>Family Dentist Phone Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     DPTBHIB-HIB_x000D_
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Booster
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMR (Measles, Mumps, Rubella)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Hepatitis B_x000D_
+</t>
+  </si>
+  <si>
+    <t>Always check the food label</t>
+  </si>
+  <si>
+    <t>in Pets with Health Conditions</t>
+  </si>
+  <si>
+    <t>Benadryl Ultratabs</t>
+  </si>
+  <si>
+    <t>redness and swelling</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sensitivity allergic reaction</t>
+  </si>
+  <si>
+    <t>it safe to get care for my other medical conditions during this time</t>
+  </si>
+  <si>
+    <t>Mental health includes our emotional, psychological, and social well-being</t>
+  </si>
+  <si>
+    <t>current concerns and mood disturbance after diagnosis of life-threatening disease</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Are you taking your medicine this morning? ... Yes and no.</t>
+  </si>
+  <si>
+    <t>07-Jul-2020</t>
+  </si>
+  <si>
+    <t>COVID-19</t>
+  </si>
+  <si>
+    <t>Acute illness situations Bees and other stingers Included here are stings or burns</t>
+  </si>
+  <si>
+    <t>illiness cure</t>
+  </si>
+  <si>
+    <t>Illnesses &amp; Infections. Illnesses and infections. COVID-19 and your child</t>
+  </si>
+  <si>
+    <t>heart disease,cancer,lung disease,accidents</t>
+  </si>
+  <si>
+    <t>Dr.Fauchi</t>
+  </si>
+  <si>
+    <t>1800-416-211</t>
+  </si>
+  <si>
+    <t>Dr.Sana</t>
+  </si>
+  <si>
+    <t>416-233-2012</t>
+  </si>
+  <si>
+    <t>12-Jul-2020</t>
+  </si>
+  <si>
+    <t>09-Jun-2020</t>
+  </si>
+  <si>
+    <t>14-May-2020</t>
+  </si>
+  <si>
+    <t>10-Jun-2020</t>
   </si>
 </sst>
 </file>
@@ -285,7 +471,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,8 +499,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF010101"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -333,8 +532,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B084"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -357,12 +562,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -384,6 +628,67 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -740,7 +1045,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,244 +1183,483 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B51AB4E0-E11E-4626-82A7-EC5057654936}">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:BI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
+      <selection activeCell="AW4" sqref="AW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="18" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.7109375" customWidth="1"/>
+    <col min="44" max="44" width="27" customWidth="1"/>
+    <col min="45" max="45" width="25.42578125" customWidth="1"/>
+    <col min="46" max="46" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.7109375" customWidth="1"/>
+    <col min="50" max="50" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="16.85546875" customWidth="1"/>
+    <col min="52" max="52" width="17.42578125" customWidth="1"/>
+    <col min="53" max="53" width="17.28515625" customWidth="1"/>
+    <col min="54" max="55" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:61" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AG1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AH1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AK1" s="6" t="s">
         <v>59</v>
       </c>
+      <c r="AL1" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM1" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN1" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="AO1" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="AP1" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ1" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="AR1" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS1" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT1" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU1" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="AV1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="AW1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX1" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="AY1" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="AZ1" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="BA1" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="BF1" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="BG1" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="BH1" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="BI1" s="17" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+    <row r="2" spans="1:61" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="27">
+        <v>1</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="27">
+        <v>1001</v>
+      </c>
+      <c r="I2" s="10">
         <v>10</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="K2" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="N2" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="T2" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="M2" s="10">
+      <c r="U2" s="10">
         <v>2894567893</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="V2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="W2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="P2" s="10">
+      <c r="X2" s="10">
         <v>2018</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Y2" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="Z2" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="AA2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="AB2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="AC2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="AD2" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="W2" s="10">
+      <c r="AE2" s="10">
         <v>18</v>
       </c>
-      <c r="X2" s="10">
+      <c r="AF2" s="10">
         <v>7</v>
       </c>
-      <c r="Y2" s="10">
+      <c r="AG2" s="10">
         <v>85</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="AH2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AI2" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AJ2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AK2" s="7" t="s">
         <v>74</v>
+      </c>
+      <c r="AL2" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="AM2" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="AN2" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="AO2" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="AP2" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="AQ2" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="AR2" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="AS2" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT2" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU2" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV2" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="AW2" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="AX2" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY2" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="AZ2" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="BA2" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="BB2" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="BC2" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="BD2" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE2" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="BF2" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="BG2" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="BH2" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="BI2" s="22" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{4291B47A-121A-43DB-BB61-B648540D07B9}"/>
-    <hyperlink ref="O2" r:id="rId2" xr:uid="{3D9E3BB3-F39E-428D-B718-7C82B8A07217}"/>
-    <hyperlink ref="L2" r:id="rId3" xr:uid="{A70BB0FB-8A1A-4BFD-BD82-43901FBD7B6C}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{4291B47A-121A-43DB-BB61-B648540D07B9}"/>
+    <hyperlink ref="W2" r:id="rId2" xr:uid="{3D9E3BB3-F39E-428D-B718-7C82B8A07217}"/>
+    <hyperlink ref="T2" r:id="rId3" xr:uid="{A70BB0FB-8A1A-4BFD-BD82-43901FBD7B6C}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{1EEF5ECD-47BD-451E-9BA9-1EB3F8E2917E}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{8AD87E73-BA05-40CD-AFA0-6DEF197EAB51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7279F4A-13AA-42E1-A91E-9E3F9E4038CE}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>